<commit_message>
Operation notebook addde + Pivot_tables notebook updated + OpenPyxl notebook updated + Matplotlib notebook updated
</commit_message>
<xml_diff>
--- a/III_Providing/data/result/ex.xlsx
+++ b/III_Providing/data/result/ex.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="df1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="df2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="df1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="df2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD" numFmtId="165"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <name val="Calibri"/>
@@ -92,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,30 +109,38 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thick"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="17">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="6" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="11" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -490,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,158 +509,179 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col customWidth="1" max="1" min="1" width="12"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="4" min="4" width="12"/>
+    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="6" min="6" width="12"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>colA</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>colB</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>colC</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>col1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>col2</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>col3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
+        <v>44562</v>
+      </c>
+      <c r="B2" t="n">
         <v>-3</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="G2" s="4" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="5" t="n">
+        <v>44562</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="F3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="G3" s="8" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="2" t="n">
+        <v>44563</v>
+      </c>
+      <c r="B4" t="n">
         <v>-1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="F4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="G4" s="9" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="5" t="n">
+        <v>44563</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="F5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="G5" s="7" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="5" t="n">
+        <v>44564</v>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>-3</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="F6" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="G6" s="11" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -667,12 +699,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col customWidth="1" max="1" min="1" width="12"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="4" min="4" width="12"/>
+    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="6" min="6" width="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -713,19 +745,19 @@
           <t>a</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="n">
+      <c r="E2" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="11" t="n">
+      <c r="F2" s="16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -735,19 +767,19 @@
           <t>b</t>
         </is>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="12" t="n">
         <v>5</v>
       </c>
     </row>
@@ -757,23 +789,23 @@
           <t>c</t>
         </is>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="13" t="n">
         <v>40</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E4" s="15" t="n">
         <v>20</v>
       </c>
-      <c r="F4" s="11" t="n">
+      <c r="F4" s="16" t="n">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>